<commit_message>
Fixed enrollment units format
Enrollment units are now uniformly presented to the thousandths place.
</commit_message>
<xml_diff>
--- a/WorkGui/bin/Debug/LawPrereqs.xlsx
+++ b/WorkGui/bin/Debug/LawPrereqs.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
   <si>
     <t>GWID</t>
   </si>
@@ -269,21 +269,36 @@
     <t>ON TRACK</t>
   </si>
   <si>
+    <t>4.450</t>
+  </si>
+  <si>
     <t>NON-GW 2012-2013</t>
   </si>
   <si>
+    <t>1.650</t>
+  </si>
+  <si>
     <t>Fall 2013</t>
   </si>
   <si>
+    <t>0.650</t>
+  </si>
+  <si>
     <t>Spring 2014</t>
   </si>
   <si>
+    <t>0.800</t>
+  </si>
+  <si>
     <t>Fall 2014</t>
   </si>
   <si>
     <t>Spring 2015</t>
   </si>
   <si>
+    <t>0.700</t>
+  </si>
+  <si>
     <t>G00000002</t>
   </si>
   <si>
@@ -299,9 +314,15 @@
     <t>course 6662 in prog.</t>
   </si>
   <si>
+    <t>6.650</t>
+  </si>
+  <si>
     <t>Fall 2012</t>
   </si>
   <si>
+    <t>1.000</t>
+  </si>
+  <si>
     <t>Spring 2013</t>
   </si>
   <si>
@@ -317,9 +338,18 @@
     <t>SKILLS REQUIREMENT MET legend</t>
   </si>
   <si>
+    <t>6.150</t>
+  </si>
+  <si>
+    <t>2.000</t>
+  </si>
+  <si>
     <t>Summer 2014</t>
   </si>
   <si>
+    <t>0.350</t>
+  </si>
+  <si>
     <t>G00000004</t>
   </si>
   <si>
@@ -332,18 +362,33 @@
     <t>A+</t>
   </si>
   <si>
+    <t>6.050</t>
+  </si>
+  <si>
     <t>NON-GW Summer 2013</t>
   </si>
   <si>
+    <t>0.400</t>
+  </si>
+  <si>
+    <t>0.150</t>
+  </si>
+  <si>
     <t>G00000005</t>
   </si>
   <si>
     <t>Kashif I. Jones</t>
   </si>
   <si>
+    <t>1.400</t>
+  </si>
+  <si>
     <t>Part-time</t>
   </si>
   <si>
+    <t>0.600</t>
+  </si>
+  <si>
     <t>G00000006</t>
   </si>
   <si>
@@ -362,12 +407,18 @@
     <t>course 6660 in prog.</t>
   </si>
   <si>
+    <t>6.950</t>
+  </si>
+  <si>
     <t>Fall 2011</t>
   </si>
   <si>
     <t>Spring 2012</t>
   </si>
   <si>
+    <t>0.500</t>
+  </si>
+  <si>
     <t>Summer 2012</t>
   </si>
   <si>
@@ -380,6 +431,9 @@
     <t>course 6664 in prog.</t>
   </si>
   <si>
+    <t>6.000</t>
+  </si>
+  <si>
     <t>G00000008</t>
   </si>
   <si>
@@ -392,6 +446,9 @@
     <t>Michael Frederick Wilson</t>
   </si>
   <si>
+    <t>5.400</t>
+  </si>
+  <si>
     <t>G00000010</t>
   </si>
   <si>
@@ -425,12 +482,18 @@
     <t>course 6658 in prog.</t>
   </si>
   <si>
+    <t>5.500</t>
+  </si>
+  <si>
     <t>G00000013</t>
   </si>
   <si>
     <t>Carolyn J Martin</t>
   </si>
   <si>
+    <t>4.750</t>
+  </si>
+  <si>
     <t>G00000014</t>
   </si>
   <si>
@@ -486,6 +549,12 @@
   </si>
   <si>
     <t>WRITING REQUIREMENT MET legend</t>
+  </si>
+  <si>
+    <t>5.900</t>
+  </si>
+  <si>
+    <t>0.200</t>
   </si>
 </sst>
 </file>
@@ -960,50 +1029,50 @@
       <c r="AN2" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="AO2" s="0">
-        <v>4.4499999999999993</v>
+      <c r="AO2" s="0" t="s">
+        <v>85</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR2" s="0">
-        <v>1.65</v>
+        <v>86</v>
+      </c>
+      <c r="AR2" s="0" t="s">
+        <v>87</v>
       </c>
       <c r="AS2" s="0">
         <v>21</v>
       </c>
       <c r="AT2" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AU2" s="0">
-        <v>0.65</v>
+        <v>88</v>
+      </c>
+      <c r="AU2" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="AV2" s="0">
         <v>9</v>
       </c>
       <c r="AW2" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="AX2" s="0">
-        <v>0.8</v>
+        <v>90</v>
+      </c>
+      <c r="AX2" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="AY2" s="0">
         <v>11</v>
       </c>
       <c r="AZ2" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BA2" s="0">
-        <v>0.65</v>
+        <v>92</v>
+      </c>
+      <c r="BA2" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="BB2" s="0">
         <v>9</v>
       </c>
       <c r="BC2" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BD2" s="0">
-        <v>0.7</v>
+        <v>93</v>
+      </c>
+      <c r="BD2" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="BE2" s="0">
         <v>10</v>
@@ -1011,19 +1080,19 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>76</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>76</v>
@@ -1035,7 +1104,7 @@
         <v>76</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>76</v>
@@ -1047,37 +1116,37 @@
         <v>76</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="N3" s="0" t="s">
         <v>76</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="P3" s="0" t="s">
         <v>76</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R3" s="0" t="s">
         <v>76</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="T3" s="0" t="s">
         <v>76</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="V3" s="0" t="s">
         <v>76</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="X3" s="0" t="s">
         <v>76</v>
@@ -1119,7 +1188,7 @@
         <v>84</v>
       </c>
       <c r="AK3" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="AL3" s="0" t="s">
         <v>84</v>
@@ -1130,68 +1199,68 @@
       <c r="AN3" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO3" s="0">
-        <v>6.65</v>
+      <c r="AO3" s="0" t="s">
+        <v>100</v>
       </c>
       <c r="AQ3" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="AR3" s="0">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="AR3" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AS3" s="0">
         <v>15</v>
       </c>
       <c r="AT3" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="AU3" s="0">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="AU3" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AV3" s="0">
         <v>15</v>
       </c>
       <c r="AW3" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="AX3" s="0">
-        <v>0.65</v>
+        <v>104</v>
+      </c>
+      <c r="AX3" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="AY3" s="0">
         <v>9</v>
       </c>
       <c r="AZ3" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="BA3" s="0">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="BA3" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB3" s="0">
         <v>13</v>
       </c>
       <c r="BC3" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="BD3" s="0">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="BD3" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE3" s="0">
         <v>12</v>
       </c>
       <c r="BF3" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BG3" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BG3" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BH3" s="0">
         <v>13</v>
       </c>
       <c r="BI3" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BJ3" s="0">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="BJ3" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BK3" s="0">
         <v>12</v>
@@ -1199,13 +1268,13 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>76</v>
@@ -1301,7 +1370,7 @@
         <v>76</v>
       </c>
       <c r="AI4" s="0" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="AJ4" s="0" t="s">
         <v>80</v>
@@ -1318,59 +1387,59 @@
       <c r="AN4" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO4" s="0">
-        <v>6.1499999999999995</v>
+      <c r="AO4" s="0" t="s">
+        <v>108</v>
       </c>
       <c r="AQ4" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR4" s="0">
-        <v>2</v>
+        <v>86</v>
+      </c>
+      <c r="AR4" s="0" t="s">
+        <v>109</v>
       </c>
       <c r="AS4" s="0">
         <v>28</v>
       </c>
       <c r="AT4" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AU4" s="0">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="AU4" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AV4" s="0">
         <v>14</v>
       </c>
       <c r="AW4" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="AX4" s="0">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="AX4" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AY4" s="0">
         <v>12</v>
       </c>
       <c r="AZ4" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="BA4" s="0">
-        <v>0.35</v>
+        <v>110</v>
+      </c>
+      <c r="BA4" s="0" t="s">
+        <v>111</v>
       </c>
       <c r="BB4" s="0">
         <v>5</v>
       </c>
       <c r="BC4" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BD4" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BD4" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE4" s="0">
         <v>12</v>
       </c>
       <c r="BF4" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BG4" s="0">
-        <v>0.8</v>
+        <v>93</v>
+      </c>
+      <c r="BG4" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="BH4" s="0">
         <v>11</v>
@@ -1378,19 +1447,19 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>76</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>76</v>
@@ -1402,7 +1471,7 @@
         <v>76</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>76</v>
@@ -1414,43 +1483,43 @@
         <v>76</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="N5" s="0" t="s">
         <v>76</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="P5" s="0" t="s">
         <v>76</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="R5" s="0" t="s">
         <v>76</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="T5" s="0" t="s">
         <v>76</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="V5" s="0" t="s">
         <v>76</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="X5" s="0" t="s">
         <v>76</v>
       </c>
       <c r="Y5" s="0" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="Z5" s="0" t="s">
         <v>84</v>
@@ -1497,77 +1566,77 @@
       <c r="AN5" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO5" s="0">
-        <v>6.0500000000000007</v>
+      <c r="AO5" s="0" t="s">
+        <v>116</v>
       </c>
       <c r="AQ5" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="AR5" s="0">
-        <v>0.4</v>
+        <v>117</v>
+      </c>
+      <c r="AR5" s="0" t="s">
+        <v>118</v>
       </c>
       <c r="AS5" s="0">
         <v>6</v>
       </c>
       <c r="AT5" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="AU5" s="0">
-        <v>0.8</v>
+        <v>101</v>
+      </c>
+      <c r="AU5" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="AV5" s="0">
         <v>11</v>
       </c>
       <c r="AW5" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="AX5" s="0">
-        <v>0.7</v>
+        <v>103</v>
+      </c>
+      <c r="AX5" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="AY5" s="0">
         <v>10</v>
       </c>
       <c r="AZ5" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="BA5" s="0">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="BA5" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB5" s="0">
         <v>14</v>
       </c>
       <c r="BC5" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="BD5" s="0">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="BD5" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE5" s="0">
         <v>15</v>
       </c>
       <c r="BF5" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="BG5" s="0">
-        <v>0.15</v>
+        <v>110</v>
+      </c>
+      <c r="BG5" s="0" t="s">
+        <v>119</v>
       </c>
       <c r="BH5" s="0">
         <v>2</v>
       </c>
       <c r="BI5" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BJ5" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BJ5" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BK5" s="0">
         <v>13</v>
       </c>
       <c r="BL5" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BM5" s="0">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="BM5" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BN5" s="0">
         <v>14</v>
@@ -1575,13 +1644,13 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>80</v>
@@ -1694,26 +1763,26 @@
       <c r="AN6" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="AO6" s="0">
-        <v>1.4</v>
+      <c r="AO6" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="AP6" s="0" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="AQ6" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="AR6" s="0">
-        <v>0.6</v>
+        <v>92</v>
+      </c>
+      <c r="AR6" s="0" t="s">
+        <v>124</v>
       </c>
       <c r="AS6" s="0">
         <v>8</v>
       </c>
       <c r="AT6" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="AU6" s="0">
-        <v>0.8</v>
+        <v>93</v>
+      </c>
+      <c r="AU6" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="AV6" s="0">
         <v>11</v>
@@ -1721,13 +1790,13 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>76</v>
@@ -1739,7 +1808,7 @@
         <v>76</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>76</v>
@@ -1751,19 +1820,19 @@
         <v>76</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="L7" s="0" t="s">
         <v>76</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="N7" s="0" t="s">
         <v>76</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="P7" s="0" t="s">
         <v>76</v>
@@ -1775,13 +1844,13 @@
         <v>76</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="T7" s="0" t="s">
         <v>76</v>
       </c>
       <c r="U7" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="V7" s="0" t="s">
         <v>76</v>
@@ -1793,7 +1862,7 @@
         <v>84</v>
       </c>
       <c r="Y7" s="0" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="Z7" s="0" t="s">
         <v>84</v>
@@ -1829,7 +1898,7 @@
         <v>84</v>
       </c>
       <c r="AK7" s="0" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="AL7" s="0" t="s">
         <v>84</v>
@@ -1840,86 +1909,86 @@
       <c r="AN7" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO7" s="0">
-        <v>6.95</v>
+      <c r="AO7" s="0" t="s">
+        <v>131</v>
       </c>
       <c r="AQ7" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="AR7" s="0">
-        <v>0.6</v>
+        <v>132</v>
+      </c>
+      <c r="AR7" s="0" t="s">
+        <v>124</v>
       </c>
       <c r="AS7" s="0">
         <v>8</v>
       </c>
       <c r="AT7" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="AU7" s="0">
-        <v>0.5</v>
+        <v>133</v>
+      </c>
+      <c r="AU7" s="0" t="s">
+        <v>134</v>
       </c>
       <c r="AV7" s="0">
         <v>7</v>
       </c>
       <c r="AW7" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="AX7" s="0">
-        <v>0.35</v>
+        <v>135</v>
+      </c>
+      <c r="AX7" s="0" t="s">
+        <v>111</v>
       </c>
       <c r="AY7" s="0">
         <v>5</v>
       </c>
       <c r="AZ7" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="BA7" s="0">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="BA7" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB7" s="0">
         <v>13</v>
       </c>
       <c r="BC7" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="BD7" s="0">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="BD7" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE7" s="0">
         <v>15</v>
       </c>
       <c r="BF7" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="BG7" s="0">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="BG7" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BH7" s="0">
         <v>12</v>
       </c>
       <c r="BI7" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="BJ7" s="0">
-        <v>0.5</v>
+        <v>90</v>
+      </c>
+      <c r="BJ7" s="0" t="s">
+        <v>134</v>
       </c>
       <c r="BK7" s="0">
         <v>7</v>
       </c>
       <c r="BL7" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BM7" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BM7" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BN7" s="0">
         <v>13</v>
       </c>
       <c r="BO7" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BP7" s="0">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="BP7" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BQ7" s="0">
         <v>15</v>
@@ -1927,31 +1996,31 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>76</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>76</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>76</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="J8" s="0" t="s">
         <v>76</v>
@@ -1963,7 +2032,7 @@
         <v>76</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="N8" s="0" t="s">
         <v>76</v>
@@ -1975,7 +2044,7 @@
         <v>76</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="R8" s="0" t="s">
         <v>76</v>
@@ -1987,7 +2056,7 @@
         <v>76</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="V8" s="0" t="s">
         <v>76</v>
@@ -2035,7 +2104,7 @@
         <v>84</v>
       </c>
       <c r="AK8" s="0" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="AL8" s="0" t="s">
         <v>84</v>
@@ -2046,59 +2115,59 @@
       <c r="AN8" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO8" s="0">
-        <v>6</v>
+      <c r="AO8" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="AQ8" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="AR8" s="0">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="AR8" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AS8" s="0">
         <v>15</v>
       </c>
       <c r="AT8" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="AU8" s="0">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="AU8" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AV8" s="0">
         <v>15</v>
       </c>
       <c r="AW8" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AX8" s="0">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="AX8" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AY8" s="0">
         <v>14</v>
       </c>
       <c r="AZ8" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="BA8" s="0">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="BA8" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB8" s="0">
         <v>13</v>
       </c>
       <c r="BC8" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BD8" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BD8" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE8" s="0">
         <v>15</v>
       </c>
       <c r="BF8" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BG8" s="0">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="BG8" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BH8" s="0">
         <v>13</v>
@@ -2106,13 +2175,13 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>76</v>
@@ -2178,7 +2247,7 @@
         <v>76</v>
       </c>
       <c r="Y9" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="Z9" s="0" t="s">
         <v>84</v>
@@ -2208,7 +2277,7 @@
         <v>76</v>
       </c>
       <c r="AI9" s="0" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="AJ9" s="0" t="s">
         <v>80</v>
@@ -2225,50 +2294,50 @@
       <c r="AN9" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO9" s="0">
-        <v>6</v>
+      <c r="AO9" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="AQ9" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR9" s="0">
-        <v>2</v>
+        <v>86</v>
+      </c>
+      <c r="AR9" s="0" t="s">
+        <v>109</v>
       </c>
       <c r="AS9" s="0">
         <v>28</v>
       </c>
       <c r="AT9" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AU9" s="0">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="AU9" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AV9" s="0">
         <v>14</v>
       </c>
       <c r="AW9" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="AX9" s="0">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="AX9" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AY9" s="0">
         <v>14</v>
       </c>
       <c r="AZ9" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BA9" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BA9" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB9" s="0">
         <v>13</v>
       </c>
       <c r="BC9" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BD9" s="0">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="BD9" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE9" s="0">
         <v>15</v>
@@ -2276,19 +2345,19 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>76</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>76</v>
@@ -2318,19 +2387,19 @@
         <v>76</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="P10" s="0" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R10" s="0" t="s">
         <v>76</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="T10" s="0" t="s">
         <v>76</v>
@@ -2348,7 +2417,7 @@
         <v>84</v>
       </c>
       <c r="Y10" s="0" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="Z10" s="0" t="s">
         <v>80</v>
@@ -2395,59 +2464,59 @@
       <c r="AN10" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="AO10" s="0">
-        <v>5.4</v>
+      <c r="AO10" s="0" t="s">
+        <v>144</v>
       </c>
       <c r="AQ10" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="AR10" s="0">
-        <v>1</v>
+        <v>132</v>
+      </c>
+      <c r="AR10" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AS10" s="0">
         <v>15</v>
       </c>
       <c r="AT10" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="AU10" s="0">
-        <v>1</v>
+        <v>133</v>
+      </c>
+      <c r="AU10" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AV10" s="0">
         <v>15</v>
       </c>
       <c r="AW10" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AX10" s="0">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="AX10" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AY10" s="0">
         <v>12</v>
       </c>
       <c r="AZ10" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="BA10" s="0">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="BA10" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB10" s="0">
         <v>12</v>
       </c>
       <c r="BC10" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BD10" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BD10" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE10" s="0">
         <v>13</v>
       </c>
       <c r="BF10" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BG10" s="0">
-        <v>0.4</v>
+        <v>93</v>
+      </c>
+      <c r="BG10" s="0" t="s">
+        <v>118</v>
       </c>
       <c r="BH10" s="0">
         <v>6</v>
@@ -2455,49 +2524,49 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>84</v>
       </c>
       <c r="C11" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>112</v>
-      </c>
       <c r="H11" s="0" t="s">
         <v>76</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="J11" s="0" t="s">
         <v>76</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="L11" s="0" t="s">
         <v>76</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="N11" s="0" t="s">
         <v>76</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="P11" s="0" t="s">
         <v>76</v>
@@ -2509,7 +2578,7 @@
         <v>76</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="T11" s="0" t="s">
         <v>76</v>
@@ -2521,13 +2590,13 @@
         <v>76</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="X11" s="0" t="s">
         <v>84</v>
       </c>
       <c r="Y11" s="0" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="Z11" s="0" t="s">
         <v>84</v>
@@ -2557,13 +2626,13 @@
         <v>84</v>
       </c>
       <c r="AI11" s="0" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="AJ11" s="0" t="s">
         <v>84</v>
       </c>
       <c r="AK11" s="0" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="AL11" s="0" t="s">
         <v>84</v>
@@ -2574,59 +2643,59 @@
       <c r="AN11" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO11" s="0">
-        <v>6</v>
+      <c r="AO11" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="AQ11" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="AR11" s="0">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="AR11" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AS11" s="0">
         <v>15</v>
       </c>
       <c r="AT11" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="AU11" s="0">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="AU11" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AV11" s="0">
         <v>15</v>
       </c>
       <c r="AW11" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AX11" s="0">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="AX11" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AY11" s="0">
         <v>15</v>
       </c>
       <c r="AZ11" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="BA11" s="0">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="BA11" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB11" s="0">
         <v>12</v>
       </c>
       <c r="BC11" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BD11" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BD11" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE11" s="0">
         <v>13</v>
       </c>
       <c r="BF11" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BG11" s="0">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="BG11" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BH11" s="0">
         <v>14</v>
@@ -2634,25 +2703,25 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>84</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>76</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>76</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>76</v>
@@ -2670,7 +2739,7 @@
         <v>76</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="N12" s="0" t="s">
         <v>76</v>
@@ -2688,13 +2757,13 @@
         <v>76</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="T12" s="0" t="s">
         <v>76</v>
       </c>
       <c r="U12" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="V12" s="0" t="s">
         <v>76</v>
@@ -2706,7 +2775,7 @@
         <v>76</v>
       </c>
       <c r="Y12" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="Z12" s="0" t="s">
         <v>84</v>
@@ -2721,28 +2790,28 @@
         <v>87</v>
       </c>
       <c r="AD12" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AE12" s="0">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AF12" s="0">
         <v>12</v>
       </c>
       <c r="AG12" s="0">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="AH12" s="0" t="s">
         <v>76</v>
       </c>
       <c r="AI12" s="0" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="AJ12" s="0" t="s">
         <v>84</v>
       </c>
       <c r="AK12" s="0" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="AL12" s="0" t="s">
         <v>84</v>
@@ -2753,59 +2822,59 @@
       <c r="AN12" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO12" s="0">
-        <v>6</v>
+      <c r="AO12" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="AQ12" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="AR12" s="0">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="AR12" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AS12" s="0">
         <v>15</v>
       </c>
       <c r="AT12" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="AU12" s="0">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="AU12" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AV12" s="0">
         <v>15</v>
       </c>
       <c r="AW12" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AX12" s="0">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="AX12" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AY12" s="0">
         <v>15</v>
       </c>
       <c r="AZ12" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="BA12" s="0">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="BA12" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB12" s="0">
         <v>15</v>
       </c>
       <c r="BC12" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BD12" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BD12" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE12" s="0">
         <v>15</v>
       </c>
       <c r="BF12" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BG12" s="0">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="BG12" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BH12" s="0">
         <v>12</v>
@@ -2813,25 +2882,25 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>76</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>76</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>76</v>
@@ -2843,19 +2912,19 @@
         <v>76</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>76</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="N13" s="0" t="s">
         <v>76</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="P13" s="0" t="s">
         <v>76</v>
@@ -2867,25 +2936,25 @@
         <v>76</v>
       </c>
       <c r="S13" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="T13" s="0" t="s">
         <v>76</v>
       </c>
       <c r="U13" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="V13" s="0" t="s">
         <v>76</v>
       </c>
       <c r="W13" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="X13" s="0" t="s">
         <v>76</v>
       </c>
       <c r="Y13" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="Z13" s="0" t="s">
         <v>80</v>
@@ -2915,13 +2984,13 @@
         <v>84</v>
       </c>
       <c r="AI13" s="0" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="AJ13" s="0" t="s">
         <v>84</v>
       </c>
       <c r="AK13" s="0" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="AL13" s="0" t="s">
         <v>84</v>
@@ -2932,59 +3001,59 @@
       <c r="AN13" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="AO13" s="0">
-        <v>5.5</v>
+      <c r="AO13" s="0" t="s">
+        <v>156</v>
       </c>
       <c r="AQ13" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="AR13" s="0">
-        <v>1</v>
+        <v>132</v>
+      </c>
+      <c r="AR13" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AS13" s="0">
         <v>15</v>
       </c>
       <c r="AT13" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="AU13" s="0">
-        <v>1</v>
+        <v>133</v>
+      </c>
+      <c r="AU13" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AV13" s="0">
         <v>15</v>
       </c>
       <c r="AW13" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="AX13" s="0">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="AX13" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AY13" s="0">
         <v>14</v>
       </c>
       <c r="AZ13" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="BA13" s="0">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="BA13" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB13" s="0">
         <v>14</v>
       </c>
       <c r="BC13" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BD13" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BD13" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE13" s="0">
         <v>12</v>
       </c>
       <c r="BF13" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BG13" s="0">
-        <v>0.5</v>
+        <v>93</v>
+      </c>
+      <c r="BG13" s="0" t="s">
+        <v>134</v>
       </c>
       <c r="BH13" s="0">
         <v>7</v>
@@ -2992,13 +3061,13 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>76</v>
@@ -3111,50 +3180,50 @@
       <c r="AN14" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="AO14" s="0">
-        <v>4.75</v>
+      <c r="AO14" s="0" t="s">
+        <v>159</v>
       </c>
       <c r="AQ14" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR14" s="0">
-        <v>2</v>
+        <v>86</v>
+      </c>
+      <c r="AR14" s="0" t="s">
+        <v>109</v>
       </c>
       <c r="AS14" s="0">
         <v>25</v>
       </c>
       <c r="AT14" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AU14" s="0">
-        <v>0.6</v>
+        <v>88</v>
+      </c>
+      <c r="AU14" s="0" t="s">
+        <v>124</v>
       </c>
       <c r="AV14" s="0">
         <v>8</v>
       </c>
       <c r="AW14" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="AX14" s="0">
-        <v>0.7</v>
+        <v>90</v>
+      </c>
+      <c r="AX14" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="AY14" s="0">
         <v>10</v>
       </c>
       <c r="AZ14" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BA14" s="0">
-        <v>0.65</v>
+        <v>92</v>
+      </c>
+      <c r="BA14" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="BB14" s="0">
         <v>9</v>
       </c>
       <c r="BC14" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BD14" s="0">
-        <v>0.8</v>
+        <v>93</v>
+      </c>
+      <c r="BD14" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="BE14" s="0">
         <v>11</v>
@@ -3162,13 +3231,13 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>76</v>
@@ -3234,7 +3303,7 @@
         <v>76</v>
       </c>
       <c r="Y15" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="Z15" s="0" t="s">
         <v>80</v>
@@ -3270,7 +3339,7 @@
         <v>84</v>
       </c>
       <c r="AK15" s="0" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="AL15" s="0" t="s">
         <v>84</v>
@@ -3281,50 +3350,50 @@
       <c r="AN15" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO15" s="0">
-        <v>6</v>
+      <c r="AO15" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="AQ15" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR15" s="0">
-        <v>2</v>
+        <v>86</v>
+      </c>
+      <c r="AR15" s="0" t="s">
+        <v>109</v>
       </c>
       <c r="AS15" s="0">
         <v>28</v>
       </c>
       <c r="AT15" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AU15" s="0">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="AU15" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AV15" s="0">
         <v>14</v>
       </c>
       <c r="AW15" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="AX15" s="0">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="AX15" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AY15" s="0">
         <v>15</v>
       </c>
       <c r="AZ15" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BA15" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BA15" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB15" s="0">
         <v>13</v>
       </c>
       <c r="BC15" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BD15" s="0">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="BD15" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE15" s="0">
         <v>13</v>
@@ -3332,13 +3401,13 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>76</v>
@@ -3404,7 +3473,7 @@
         <v>76</v>
       </c>
       <c r="Y16" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="Z16" s="0" t="s">
         <v>84</v>
@@ -3440,7 +3509,7 @@
         <v>84</v>
       </c>
       <c r="AK16" s="0" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="AL16" s="0" t="s">
         <v>84</v>
@@ -3451,50 +3520,50 @@
       <c r="AN16" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO16" s="0">
-        <v>6</v>
+      <c r="AO16" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="AQ16" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR16" s="0">
-        <v>2</v>
+        <v>86</v>
+      </c>
+      <c r="AR16" s="0" t="s">
+        <v>109</v>
       </c>
       <c r="AS16" s="0">
         <v>28</v>
       </c>
       <c r="AT16" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AU16" s="0">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="AU16" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AV16" s="0">
         <v>14</v>
       </c>
       <c r="AW16" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="AX16" s="0">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="AX16" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AY16" s="0">
         <v>15</v>
       </c>
       <c r="AZ16" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BA16" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BA16" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB16" s="0">
         <v>14</v>
       </c>
       <c r="BC16" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BD16" s="0">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="BD16" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE16" s="0">
         <v>14</v>
@@ -3502,13 +3571,13 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>84</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>76</v>
@@ -3526,37 +3595,37 @@
         <v>76</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="J17" s="0" t="s">
         <v>76</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="L17" s="0" t="s">
         <v>76</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="N17" s="0" t="s">
         <v>76</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="P17" s="0" t="s">
         <v>76</v>
       </c>
       <c r="Q17" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R17" s="0" t="s">
         <v>76</v>
       </c>
       <c r="S17" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="T17" s="0" t="s">
         <v>76</v>
@@ -3568,7 +3637,7 @@
         <v>76</v>
       </c>
       <c r="W17" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="X17" s="0" t="s">
         <v>76</v>
@@ -3604,13 +3673,13 @@
         <v>76</v>
       </c>
       <c r="AI17" s="0" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="AJ17" s="0" t="s">
         <v>84</v>
       </c>
       <c r="AK17" s="0" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="AL17" s="0" t="s">
         <v>84</v>
@@ -3621,59 +3690,59 @@
       <c r="AN17" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO17" s="0">
-        <v>6</v>
+      <c r="AO17" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="AQ17" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="AR17" s="0">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="AR17" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AS17" s="0">
         <v>15</v>
       </c>
       <c r="AT17" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="AU17" s="0">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="AU17" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AV17" s="0">
         <v>15</v>
       </c>
       <c r="AW17" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AX17" s="0">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="AX17" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AY17" s="0">
         <v>12</v>
       </c>
       <c r="AZ17" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="BA17" s="0">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="BA17" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB17" s="0">
         <v>15</v>
       </c>
       <c r="BC17" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BD17" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BD17" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE17" s="0">
         <v>15</v>
       </c>
       <c r="BF17" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BG17" s="0">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="BG17" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BH17" s="0">
         <v>12</v>
@@ -3681,25 +3750,25 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>76</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>76</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>76</v>
@@ -3717,37 +3786,37 @@
         <v>76</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="N18" s="0" t="s">
         <v>76</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="P18" s="0" t="s">
         <v>76</v>
       </c>
       <c r="Q18" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="R18" s="0" t="s">
         <v>76</v>
       </c>
       <c r="S18" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="T18" s="0" t="s">
         <v>76</v>
       </c>
       <c r="U18" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="V18" s="0" t="s">
         <v>76</v>
       </c>
       <c r="W18" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="X18" s="0" t="s">
         <v>76</v>
@@ -3783,7 +3852,7 @@
         <v>84</v>
       </c>
       <c r="AI18" s="0" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="AJ18" s="0" t="s">
         <v>80</v>
@@ -3800,59 +3869,59 @@
       <c r="AN18" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO18" s="0">
-        <v>6</v>
+      <c r="AO18" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="AQ18" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="AR18" s="0">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="AR18" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AS18" s="0">
         <v>15</v>
       </c>
       <c r="AT18" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="AU18" s="0">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="AU18" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AV18" s="0">
         <v>15</v>
       </c>
       <c r="AW18" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AX18" s="0">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="AX18" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AY18" s="0">
         <v>14</v>
       </c>
       <c r="AZ18" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="BA18" s="0">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="BA18" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB18" s="0">
         <v>12</v>
       </c>
       <c r="BC18" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BD18" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BD18" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BE18" s="0">
         <v>15</v>
       </c>
       <c r="BF18" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BG18" s="0">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="BG18" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BH18" s="0">
         <v>13</v>
@@ -3860,25 +3929,25 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>76</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>76</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>76</v>
@@ -3890,37 +3959,37 @@
         <v>76</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="L19" s="0" t="s">
         <v>76</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="N19" s="0" t="s">
         <v>76</v>
       </c>
       <c r="O19" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="P19" s="0" t="s">
         <v>80</v>
       </c>
       <c r="Q19" s="0" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="R19" s="0" t="s">
         <v>76</v>
       </c>
       <c r="S19" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="T19" s="0" t="s">
         <v>76</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="V19" s="0" t="s">
         <v>76</v>
@@ -3932,7 +4001,7 @@
         <v>84</v>
       </c>
       <c r="Y19" s="0" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="Z19" s="0" t="s">
         <v>84</v>
@@ -3962,7 +4031,7 @@
         <v>84</v>
       </c>
       <c r="AI19" s="0" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="AJ19" s="0" t="s">
         <v>80</v>
@@ -3979,68 +4048,68 @@
       <c r="AN19" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO19" s="0">
-        <v>6</v>
+      <c r="AO19" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="AQ19" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="AR19" s="0">
-        <v>1</v>
+        <v>174</v>
+      </c>
+      <c r="AR19" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AS19" s="0">
         <v>15</v>
       </c>
       <c r="AT19" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="AU19" s="0">
-        <v>1</v>
+        <v>175</v>
+      </c>
+      <c r="AU19" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="AV19" s="0">
         <v>12</v>
       </c>
       <c r="AW19" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AX19" s="0">
-        <v>0.65</v>
+        <v>88</v>
+      </c>
+      <c r="AX19" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="AY19" s="0">
         <v>9</v>
       </c>
       <c r="AZ19" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="BA19" s="0">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="BA19" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BB19" s="0">
         <v>14</v>
       </c>
       <c r="BC19" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="BD19" s="0">
-        <v>0.35</v>
+        <v>110</v>
+      </c>
+      <c r="BD19" s="0" t="s">
+        <v>111</v>
       </c>
       <c r="BE19" s="0">
         <v>5</v>
       </c>
       <c r="BF19" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BG19" s="0">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="BG19" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BH19" s="0">
         <v>14</v>
       </c>
       <c r="BI19" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BJ19" s="0">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="BJ19" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="BK19" s="0">
         <v>15</v>
@@ -4048,19 +4117,19 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>84</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>76</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>76</v>
@@ -4072,13 +4141,13 @@
         <v>76</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="J20" s="0" t="s">
         <v>76</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="L20" s="0" t="s">
         <v>76</v>
@@ -4090,7 +4159,7 @@
         <v>76</v>
       </c>
       <c r="O20" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="P20" s="0" t="s">
         <v>76</v>
@@ -4102,25 +4171,25 @@
         <v>76</v>
       </c>
       <c r="S20" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="T20" s="0" t="s">
         <v>76</v>
       </c>
       <c r="U20" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="V20" s="0" t="s">
         <v>76</v>
       </c>
       <c r="W20" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="X20" s="0" t="s">
         <v>76</v>
       </c>
       <c r="Y20" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="Z20" s="0" t="s">
         <v>84</v>
@@ -4150,13 +4219,13 @@
         <v>76</v>
       </c>
       <c r="AI20" s="0" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="AJ20" s="0" t="s">
         <v>76</v>
       </c>
       <c r="AK20" s="0" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="AL20" s="0" t="s">
         <v>84</v>
@@ -4167,89 +4236,89 @@
       <c r="AN20" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AO20" s="0">
-        <v>5.9000000000000012</v>
+      <c r="AO20" s="0" t="s">
+        <v>179</v>
       </c>
       <c r="AP20" s="0" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="AQ20" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="AR20" s="0">
-        <v>0.8</v>
+        <v>132</v>
+      </c>
+      <c r="AR20" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="AS20" s="0">
         <v>11</v>
       </c>
       <c r="AT20" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="AU20" s="0">
-        <v>0.7</v>
+        <v>133</v>
+      </c>
+      <c r="AU20" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="AV20" s="0">
         <v>10</v>
       </c>
       <c r="AW20" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="AX20" s="0">
-        <v>0.7</v>
+        <v>101</v>
+      </c>
+      <c r="AX20" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="AY20" s="0">
         <v>10</v>
       </c>
       <c r="AZ20" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="BA20" s="0">
-        <v>0.7</v>
+        <v>103</v>
+      </c>
+      <c r="BA20" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="BB20" s="0">
         <v>10</v>
       </c>
       <c r="BC20" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="BD20" s="0">
-        <v>0.7</v>
+        <v>88</v>
+      </c>
+      <c r="BD20" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="BE20" s="0">
         <v>10</v>
       </c>
       <c r="BF20" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="BG20" s="0">
-        <v>0.7</v>
+        <v>90</v>
+      </c>
+      <c r="BG20" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="BH20" s="0">
         <v>10</v>
       </c>
       <c r="BI20" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="BJ20" s="0">
-        <v>0.2</v>
+        <v>110</v>
+      </c>
+      <c r="BJ20" s="0" t="s">
+        <v>180</v>
       </c>
       <c r="BK20" s="0">
         <v>3</v>
       </c>
       <c r="BL20" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="BM20" s="0">
-        <v>0.7</v>
+        <v>92</v>
+      </c>
+      <c r="BM20" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="BN20" s="0">
         <v>10</v>
       </c>
       <c r="BO20" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BP20" s="0">
-        <v>0.7</v>
+        <v>93</v>
+      </c>
+      <c r="BP20" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="BQ20" s="0">
         <v>10</v>

</xml_diff>